<commit_message>
Updated patterns and code
</commit_message>
<xml_diff>
--- a/patternsDesign.xlsx
+++ b/patternsDesign.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JensE\Documents\ImportDocs\exjob\malPatEval\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C72AD36A-D1F7-4B69-894D-AA8F501C7A0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C3CF810-A8DF-4E44-BF81-00E3AFC5C772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="2190" windowWidth="38640" windowHeight="21120" xr2:uid="{483EB3CA-C8CE-46A0-96CF-956BBBC5F2A0}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
-  <si>
-    <t>IAM</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
   <si>
     <t>remoteAccessMFA</t>
   </si>
@@ -74,9 +71,6 @@
     <t>M1036, M1032, M1030, M1017</t>
   </si>
   <si>
-    <t>excessivePrivAccounts</t>
-  </si>
-  <si>
     <t>ATT&amp;CK Techniques</t>
   </si>
   <si>
@@ -98,9 +92,6 @@
     <t>Sensitive information (e.g., credentials, keys, tokens) stored in plaintext without encryption may be susceptible to unauthorized access and compromise.</t>
   </si>
   <si>
-    <t>Pattern abuse case</t>
-  </si>
-  <si>
     <t>Pattern name</t>
   </si>
   <si>
@@ -113,22 +104,58 @@
     <t>Group of patterns</t>
   </si>
   <si>
-    <t>Identity, Credentials</t>
-  </si>
-  <si>
-    <t>Identified [Identity] classified as low privilige  with association {highPrivAppIAMs}</t>
-  </si>
-  <si>
-    <t>Existence of service, guest or any other temporarily accounts with excessive permissions may facilitate initial access and lateral movement.</t>
-  </si>
-  <si>
     <t>Identified [Credentials] associated to an [Application] classified as a remote access service, lacking the association {ConditionalAuthentication}</t>
   </si>
   <si>
-    <t>T1199, T1078, 1078</t>
-  </si>
-  <si>
     <t>M1032, M1018, M1026, M1036</t>
+  </si>
+  <si>
+    <t>T1199, T1078</t>
+  </si>
+  <si>
+    <t>Identity &amp; Authentication</t>
+  </si>
+  <si>
+    <t>shadowAdmin</t>
+  </si>
+  <si>
+    <t>Pattern impact/abuse case</t>
+  </si>
+  <si>
+    <t>User accounts that have inadvertently been assigned admin privilige may enable attackers to control accounts with unrestricted access and movement</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>M1</t>
+  </si>
+  <si>
+    <t>Network</t>
+  </si>
+  <si>
+    <t>M2</t>
+  </si>
+  <si>
+    <t>M1,M2</t>
+  </si>
+  <si>
+    <t>highPrivServiceAccounts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identified an [Identity] classified as service account with association {highPrivAppIAMs} </t>
+  </si>
+  <si>
+    <t>Identified an [Identity] classified as not admin  with association {highPrivAppIAMs}</t>
+  </si>
+  <si>
+    <t>Identity, Priviliges</t>
+  </si>
+  <si>
+    <t>Identity, Network</t>
+  </si>
+  <si>
+    <t>Existence of service, support or any other non user accounts with excessive privileges may facilitate lateral movement and access to network resources.</t>
   </si>
 </sst>
 </file>
@@ -524,16 +551,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44032789-62F5-4A42-883C-D224EEED2797}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="A1:XFD1048576"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.77734375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="27.109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="38.33203125" style="3" customWidth="1"/>
     <col min="3" max="3" width="89.33203125" style="3" customWidth="1"/>
     <col min="4" max="4" width="63.44140625" style="3" customWidth="1"/>
     <col min="5" max="5" width="52.33203125" style="4" customWidth="1"/>
@@ -542,123 +569,158 @@
     <col min="8" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="G5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="5" t="s">
+      <c r="D16" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="5" t="s">
+      <c r="E16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="3" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-    </row>
-    <row r="14" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>